<commit_message>
remove rubber from BoM
</commit_message>
<xml_diff>
--- a/Bike Sensor Project/Hardware Bill of Materials.xlsx
+++ b/Bike Sensor Project/Hardware Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casso\Documents\Serial_and_milk\Bike Sensor Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D460158-00C2-44A5-A3CC-52B1890AB663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9E4501-C6D7-40C0-AD2D-90B4378F009D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F96A92AD-15D1-4392-9DCD-00ED13C437D1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F96A92AD-15D1-4392-9DCD-00ED13C437D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Item</t>
   </si>
@@ -138,15 +138,6 @@
   </si>
   <si>
     <t>any</t>
-  </si>
-  <si>
-    <t>Rubber</t>
-  </si>
-  <si>
-    <t>to compress between bike rack and enclosure. We used ninjaflex 3D print filament</t>
-  </si>
-  <si>
-    <t>to compress to bike rack</t>
   </si>
 </sst>
 </file>
@@ -512,7 +503,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,17 +670,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>

</xml_diff>